<commit_message>
Practice testng Listenter 27 January
</commit_message>
<xml_diff>
--- a/SeleniumPracticeProject/src/main/java/com/crm/qa/testdata/ExcelTestDataFile.xlsx
+++ b/SeleniumPracticeProject/src/main/java/com/crm/qa/testdata/ExcelTestDataFile.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>First Name</t>
   </si>
@@ -445,7 +445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -568,10 +568,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -592,6 +592,14 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>